<commit_message>
Fix "Major" Physics and Math
</commit_message>
<xml_diff>
--- a/FinalProject/Codebase/datasource/ds.xlsx
+++ b/FinalProject/Codebase/datasource/ds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angelapaiva/Documents/Data Science Course - UoT/FinalProject/Codebase/datasource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F5CC07-596B-AF42-A886-162DDF5B0394}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644D7688-04C6-F847-ADB8-63876D6A5625}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="70">
   <si>
     <t>JobTitle</t>
   </si>
@@ -194,9 +194,6 @@
   </si>
   <si>
     <t>Quantitative Finance</t>
-  </si>
-  <si>
-    <t>major</t>
   </si>
   <si>
     <t>Biostatistics</t>
@@ -668,7 +665,7 @@
   <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -691,7 +688,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -708,7 +705,7 @@
         <v>14</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -725,7 +722,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -742,7 +739,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -759,7 +756,7 @@
         <v>6</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -776,7 +773,7 @@
         <v>6</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -793,7 +790,7 @@
         <v>6</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -801,16 +798,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -827,7 +824,7 @@
         <v>6</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -844,7 +841,7 @@
         <v>54</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -861,7 +858,7 @@
         <v>6</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -875,10 +872,10 @@
         <v>13</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -895,7 +892,7 @@
         <v>6</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -912,7 +909,7 @@
         <v>11</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -929,7 +926,7 @@
         <v>11</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -946,7 +943,7 @@
         <v>6</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -963,7 +960,7 @@
         <v>6</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -980,7 +977,7 @@
         <v>23</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -997,7 +994,7 @@
         <v>6</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1014,7 +1011,7 @@
         <v>6</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1031,7 +1028,7 @@
         <v>6</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1048,7 +1045,7 @@
         <v>6</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1065,7 +1062,7 @@
         <v>6</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1082,7 +1079,7 @@
         <v>6</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1099,7 +1096,7 @@
         <v>6</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1116,7 +1113,7 @@
         <v>11</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1133,7 +1130,7 @@
         <v>54</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1150,7 +1147,7 @@
         <v>54</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1167,7 +1164,7 @@
         <v>6</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1184,7 +1181,7 @@
         <v>6</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1201,7 +1198,7 @@
         <v>6</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1218,7 +1215,7 @@
         <v>6</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1235,7 +1232,7 @@
         <v>6</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1252,7 +1249,7 @@
         <v>6</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1269,7 +1266,7 @@
         <v>11</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1286,7 +1283,7 @@
         <v>6</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1303,7 +1300,7 @@
         <v>6</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1317,10 +1314,10 @@
         <v>13</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1337,7 +1334,7 @@
         <v>6</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1354,7 +1351,7 @@
         <v>23</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1371,7 +1368,7 @@
         <v>23</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1388,7 +1385,7 @@
         <v>6</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1405,7 +1402,7 @@
         <v>6</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1413,7 +1410,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>13</v>
@@ -1422,7 +1419,7 @@
         <v>6</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1439,7 +1436,7 @@
         <v>6</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1456,7 +1453,7 @@
         <v>6</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1473,7 +1470,7 @@
         <v>6</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1490,7 +1487,7 @@
         <v>6</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1507,7 +1504,7 @@
         <v>6</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1524,7 +1521,7 @@
         <v>54</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1541,7 +1538,7 @@
         <v>54</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1558,7 +1555,7 @@
         <v>54</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1566,7 +1563,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>13</v>
@@ -1575,7 +1572,7 @@
         <v>54</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1583,7 +1580,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>13</v>
@@ -1592,7 +1589,7 @@
         <v>54</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1600,7 +1597,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>13</v>
@@ -1609,7 +1606,7 @@
         <v>11</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1617,7 +1614,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>13</v>
@@ -1626,7 +1623,7 @@
         <v>6</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1634,7 +1631,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>13</v>
@@ -1643,7 +1640,7 @@
         <v>6</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1651,7 +1648,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>13</v>
@@ -1660,7 +1657,7 @@
         <v>6</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1668,7 +1665,7 @@
         <v>57</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>13</v>
@@ -1677,7 +1674,7 @@
         <v>6</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>